<commit_message>
script compiler moved to botium
</commit_message>
<xml_diff>
--- a/samples/xlsx/spec/convo/Vorlage_Test_Bot.xlsx
+++ b/samples/xlsx/spec/convo/Vorlage_Test_Bot.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\avfs03.at-work.local\Home_VIE\knoglejo\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="9795" activeTab="2"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>User</t>
   </si>
@@ -71,9 +66,6 @@
     <t>Tarif</t>
   </si>
   <si>
-    <t>Für viele Tarife ist ein Tarifwechsel in der 3Kundenzone möglich. Bitte beachten Sie, dass Sie ab 6 Monate vor Ende Ihrer Mindestvertragsdauer auf einen Tarif innerhalb derselben oder zu einer niedrigeren Tarifgruppe wechseln können. Natürlich bleibt Ihre Rufnummer bei einem Tarifwechsel bestehen.Ein Tarifwechsel in eine höhere Tarifgruppe ist jederzeit möglich. Ihre aktuelle Tarifgruppe finden Sie ebenfalls in der 3Kundenzone. Ein Tarifwechsel wird immer erst zur nächsten Rechnungsperiode gültig. Ein Tarifwechsel von Sprach- auf Datentarif und umgekehrt ist nicht möglich. Können Sie den Tarifwechsel nicht in Ihrer 3Kundenzone durchführen oder haben Sie Fragen dann wenden Sie sich bitte an unser 3Service-Team.</t>
-  </si>
-  <si>
     <t>Zusatzpaket-Vertrag</t>
   </si>
   <si>
@@ -83,60 +75,9 @@
     <t>3Service-Team kontaktieren</t>
   </si>
   <si>
-    <t>Hier können Sie das 3Service-Team anrufen</t>
-  </si>
-  <si>
     <t>Netz</t>
   </si>
   <si>
-    <t>Es tut uns leid, dass Sie mit unserem Netz nicht zufrieden sind. Es kann vorkommen, dass an manchen Orten das 3Netz aus verschiedenen Gründen manchmal nicht optimal funktioniert oder Ihr Gerät nicht ideal eingestellt ist – bitte kontaktieren Sie meine Kollegen aus dem 3Service-Team, damit sie wir Ihren Fall individuell prüfen können. Möchten Sie das 3Service-Team kontaktieren?</t>
-  </si>
-  <si>
-    <r>
-      <t>Wenn Sie Ihren Vertrag kündigen möchten, beachten Sie bitte die laut AGB gültige Kündigungsfrist und bei Handy-Tarifen Ihre Mindestvertragsdauer. Details hierzu finden Sie auf Ihrem Servicevertrag oder in der </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF2E7FAC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3Kundenzone</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF373A3C"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Ihr Kündigungsschreiben schicken Sie uns bitte per Post, Fax oder nutzen Sie hierfür das </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF2E7FAC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Kontaktformular</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF373A3C"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Sterbefall</t>
   </si>
   <si>
@@ -146,18 +87,9 @@
     <t>Vertrag auflösen</t>
   </si>
   <si>
-    <t>Um den Vertrag aufzulösen, lassen Sie uns bitte nur noch die Sterbeurkunde zukommen. Nach einer kurzen Prüfung, ob alle Rechnungen beglichen wurden, lösen wir den Service-Vertrag für Sie auf. Sie können uns die Sterbeurkunde auf einem der folgenden Wege zukommen lassen:
-Link zum Kontaktformular
-Post/Fax-Kontaktdaten
-Per E-Mail an serviceteam(@)drei.at</t>
-  </si>
-  <si>
     <t>Zusatzpaket schriftlich kündigen</t>
   </si>
   <si>
-    <t>Wenn Sie Ihr Zusatzpaket schriftlich kündigen möchten, beachten Sie bitte die gültige Kündigungsfrist und gegebenenfalls die Bindefrist Ihres Zusatzpaketes. Details hierzu finden Sie auf Ihrem Servicevertrag oder in der 3Kundenzone . Ihr Kündigungsschreiben schicken Sie uns bitte per Post, Fax oder nutzen Sie hierfür das Kontaktformular.</t>
-  </si>
-  <si>
     <t>Umzug ins Ausland</t>
   </si>
   <si>
@@ -167,29 +99,44 @@
     <t>vorzeitige Endabrechnung</t>
   </si>
   <si>
-    <t>Möchten Sie unsere Dienste nach Ihrem Umzug nicht mehr nutzen, ziehen wir ganz einfach die Endabrechnung mit allen ausstehenden Grundentgelten vor. Lassen Sie uns wissen, zu welchem Datum das passieren soll. Ihr Kündigungsschreiben können Sie uns auf folgendem Weg übermitteln:</t>
-  </si>
-  <si>
     <t>per Post/Fax</t>
   </si>
   <si>
-    <t>Link zur Kontaktseite</t>
-  </si>
-  <si>
     <t>Anderer Grund</t>
   </si>
   <si>
     <t>Ich wäre froh, wenn Sie Kunde bei Drei bleiben würden. Vielleicht können wir für Ihren Kündigungsgrund eine Lösung finden. Möchten Sie mit meinen Kollegen im 3Service-Team darüber sprechen?</t>
   </si>
   <si>
-    <t>Wenn Sie Ihren Vertrag kündigen möchten, beachten Sie bitte die laut AGB gültige Kündigungsfrist und bei Handy-Tarifen Ihre Mindestvertragsdauer. Details hierzu finden Sie auf Ihrem Servicevertrag oder in der 3Kundenzone. Ihr Kündigungsschreiben schicken Sie uns bitte per Post, Fax oder nutzen Sie hierfür das Kontaktformular .</t>
+    <t>Um den Vertrag aufzulösen, lassen Sie uns bitte nur noch die Sterbeurkunde zukommen. Nach einer kurzen Prüfung, ob alle Rechnungen beglichen wurden, lösen wir den Service-Vertrag für Sie auf. Sie können uns die Sterbeurkunde auf einem der folgenden Wege zukommen lassen:</t>
+  </si>
+  <si>
+    <t>Möchten Sie unsere Dienste nach Ihrem Umzug nicht mehr nutzen, ziehen wir ganz einfach die Endabrechnung mit allen ausstehenden Grundentgelten vor. Lassen Sie uns wissen, zu welchem Datum das passieren soll.  Ihr Kündigungsschreiben können Sie uns auf folgendem Weg übermitteln:</t>
+  </si>
+  <si>
+    <t>Wenn Sie Ihren Vertrag kündigen möchten, beachten Sie bitte die laut AGB gültige Kündigungsfrist und bei Handy-Tarifen Ihre Mindestvertragsdauer. Details hierzu finden Sie auf Ihrem Servicevertrag oder in der 3Kundenzone. Ihr Kündigungsschreiben schicken Sie uns bitte per Post, Fax oder nutzen Sie hierfür das Kontaktformular .</t>
+  </si>
+  <si>
+    <t>Wenn Sie Ihr Zusatzpaket schriftlich kündigen möchten, beachten Sie bitte die gültige Kündigungsfrist und gegebenenfalls die Bindefrist Ihres Zusatzpaketes. Details hierzu finden Sie auf Ihrem Servicevertrag oder in der 3Kundenzone . Ihr Kündigungsschreiben schicken Sie uns bitte per Post, Fax oder nutzen Sie hierfür das Kontaktformular.</t>
+  </si>
+  <si>
+    <t>Es tut uns leid, dass Sie mit unserem Netz nicht zufrieden sind.  Es kann vorkommen, dass an manchen Orten das 3Netz aus verschiedenen Gründen manchmal nicht optimal funktioniert oder Ihr Gerät nicht ideal eingestellt ist – bitte kontaktieren Sie meine Kollegen aus dem 3Service-Team, damit sie wir Ihren Fall individuell prüfen können. Möchten Sie das 3Service-Team kontaktieren?</t>
+  </si>
+  <si>
+    <t>Hier können Sie das 3Service-Team anrufen</t>
+  </si>
+  <si>
+    <t>Für viele Tarife ist ein Tarifwechsel in der  3Kundenzone möglich. Bitte beachten Sie, dass Sie ab 6 Monate vor Ende Ihrer Mindestvertragsdauer auf einen Tarif innerhalb derselben oder zu einer niedrigeren Tarifgruppe wechseln können. Natürlich bleibt Ihre Rufnummer bei einem Tarifwechsel bestehen.    Ein Tarifwechsel in eine höhere Tarifgruppe ist jederzeit möglich. Ihre aktuelle Tarifgruppe finden Sie ebenfalls in der  3Kundenzone. Ein Tarifwechsel wird immer erst zur nächsten Rechnungsperiode gültig. Ein Tarifwechsel von Sprach- auf Datentarif und umgekehrt ist nicht möglich.      Können Sie den Tarifwechsel nicht in Ihrer 3Kundenzone durchführen oder haben Sie Fragen dann wenden Sie sich bitte an unser  3Service-Team.</t>
+  </si>
+  <si>
+    <t>Ich verstehe, Sie wollen uns kontaktieren.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,21 +154,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF373A3C"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF2E7FAC"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,12 +224,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -312,9 +245,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -352,9 +285,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,7 +322,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,7 +357,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -604,7 +537,7 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="42.7109375" customWidth="1"/>
   </cols>
@@ -630,7 +563,7 @@
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="46.28515625" customWidth="1"/>
   </cols>
@@ -652,11 +585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" style="2" customWidth="1"/>
@@ -774,7 +707,7 @@
     <row r="19" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,26 +728,26 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -847,14 +780,14 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B32" s="4"/>
     </row>
-    <row r="33" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,10 +796,10 @@
       </c>
       <c r="B34" s="4"/>
     </row>
-    <row r="35" spans="1:2" ht="138" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,26 +832,26 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B41" s="4"/>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B43" s="4"/>
     </row>
-    <row r="44" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,26 +872,26 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" s="4"/>
     </row>
     <row r="49" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B50" s="4"/>
     </row>
-    <row r="51" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -991,38 +924,38 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B57" s="4"/>
     </row>
     <row r="58" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B59" s="4"/>
     </row>
     <row r="60" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B61" s="4"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,14 +988,14 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B68" s="4"/>
     </row>
-    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1074,7 +1007,7 @@
     <row r="71" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>